<commit_message>
Multiply actual emission change in with 100 in backend instead of in frontend, to be consistent with needed emission change in percent
</commit_message>
<xml_diff>
--- a/data/tests/reference_dataframes/df_actual_change_percent.xlsx
+++ b/data/tests/reference_dataframes/df_actual_change_percent.xlsx
@@ -595,7 +595,7 @@
         </is>
       </c>
       <c r="V2" t="n">
-        <v>0.006777828626744745</v>
+        <v>0.6777828626744745</v>
       </c>
     </row>
     <row r="3">
@@ -675,7 +675,7 @@
         </is>
       </c>
       <c r="V3" t="n">
-        <v>-0.0287830460823655</v>
+        <v>-2.87830460823655</v>
       </c>
     </row>
     <row r="4">
@@ -755,7 +755,7 @@
         </is>
       </c>
       <c r="V4" t="n">
-        <v>-0.03106354699703534</v>
+        <v>-3.106354699703534</v>
       </c>
     </row>
     <row r="5">
@@ -835,7 +835,7 @@
         </is>
       </c>
       <c r="V5" t="n">
-        <v>-0.01574180862670948</v>
+        <v>-1.574180862670948</v>
       </c>
     </row>
     <row r="6">
@@ -915,7 +915,7 @@
         </is>
       </c>
       <c r="V6" t="n">
-        <v>-0.0178675368142107</v>
+        <v>-1.78675368142107</v>
       </c>
     </row>
     <row r="7">
@@ -995,7 +995,7 @@
         </is>
       </c>
       <c r="V7" t="n">
-        <v>-0.05216881594416081</v>
+        <v>-5.216881594416081</v>
       </c>
     </row>
     <row r="8">
@@ -1075,7 +1075,7 @@
         </is>
       </c>
       <c r="V8" t="n">
-        <v>-0.01616468362625644</v>
+        <v>-1.616468362625644</v>
       </c>
     </row>
     <row r="9">
@@ -1155,7 +1155,7 @@
         </is>
       </c>
       <c r="V9" t="n">
-        <v>-0.01644157684384816</v>
+        <v>-1.644157684384816</v>
       </c>
     </row>
     <row r="10">
@@ -1235,7 +1235,7 @@
         </is>
       </c>
       <c r="V10" t="n">
-        <v>0.02436271158385382</v>
+        <v>2.436271158385382</v>
       </c>
     </row>
     <row r="11">
@@ -1315,7 +1315,7 @@
         </is>
       </c>
       <c r="V11" t="n">
-        <v>-0.0009299141160527211</v>
+        <v>-0.09299141160527212</v>
       </c>
     </row>
     <row r="12">
@@ -1395,7 +1395,7 @@
         </is>
       </c>
       <c r="V12" t="n">
-        <v>-0.01882506843830222</v>
+        <v>-1.882506843830222</v>
       </c>
     </row>
     <row r="13">
@@ -1475,7 +1475,7 @@
         </is>
       </c>
       <c r="V13" t="n">
-        <v>-0.08455961710818204</v>
+        <v>-8.455961710818203</v>
       </c>
     </row>
     <row r="14">
@@ -1555,7 +1555,7 @@
         </is>
       </c>
       <c r="V14" t="n">
-        <v>-0.01334166669638212</v>
+        <v>-1.334166669638212</v>
       </c>
     </row>
     <row r="15">
@@ -1635,7 +1635,7 @@
         </is>
       </c>
       <c r="V15" t="n">
-        <v>-0.04490451877030514</v>
+        <v>-4.490451877030513</v>
       </c>
     </row>
     <row r="16">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="V16" t="n">
-        <v>0.02845237355137667</v>
+        <v>2.845237355137667</v>
       </c>
     </row>
     <row r="17">
@@ -1795,7 +1795,7 @@
         </is>
       </c>
       <c r="V17" t="n">
-        <v>0.0004800095132785536</v>
+        <v>0.04800095132785536</v>
       </c>
     </row>
     <row r="18">
@@ -1875,7 +1875,7 @@
         </is>
       </c>
       <c r="V18" t="n">
-        <v>-0.0198036971037208</v>
+        <v>-1.980369710372081</v>
       </c>
     </row>
     <row r="19">
@@ -1955,7 +1955,7 @@
         </is>
       </c>
       <c r="V19" t="n">
-        <v>-0.03134109373275062</v>
+        <v>-3.134109373275062</v>
       </c>
     </row>
     <row r="20">
@@ -2035,7 +2035,7 @@
         </is>
       </c>
       <c r="V20" t="n">
-        <v>-0.01812206297325211</v>
+        <v>-1.812206297325211</v>
       </c>
     </row>
     <row r="21">
@@ -2115,7 +2115,7 @@
         </is>
       </c>
       <c r="V21" t="n">
-        <v>-0.02186800053113524</v>
+        <v>-2.186800053113524</v>
       </c>
     </row>
     <row r="22">
@@ -2195,7 +2195,7 @@
         </is>
       </c>
       <c r="V22" t="n">
-        <v>-0.04366957800173508</v>
+        <v>-4.366957800173508</v>
       </c>
     </row>
     <row r="23">
@@ -2275,7 +2275,7 @@
         </is>
       </c>
       <c r="V23" t="n">
-        <v>-0.01357684952033877</v>
+        <v>-1.357684952033877</v>
       </c>
     </row>
     <row r="24">
@@ -2355,7 +2355,7 @@
         </is>
       </c>
       <c r="V24" t="n">
-        <v>-0.01854131169923561</v>
+        <v>-1.854131169923561</v>
       </c>
     </row>
     <row r="25">
@@ -2435,7 +2435,7 @@
         </is>
       </c>
       <c r="V25" t="n">
-        <v>-0.05591413142280759</v>
+        <v>-5.59141314228076</v>
       </c>
     </row>
     <row r="26">
@@ -2515,7 +2515,7 @@
         </is>
       </c>
       <c r="V26" t="n">
-        <v>-0.06208913878116392</v>
+        <v>-6.208913878116392</v>
       </c>
     </row>
     <row r="27">
@@ -2595,7 +2595,7 @@
         </is>
       </c>
       <c r="V27" t="n">
-        <v>-0.03300449527495998</v>
+        <v>-3.300449527495998</v>
       </c>
     </row>
     <row r="28">
@@ -2675,7 +2675,7 @@
         </is>
       </c>
       <c r="V28" t="n">
-        <v>-0.02638673933704393</v>
+        <v>-2.638673933704393</v>
       </c>
     </row>
     <row r="29">
@@ -2755,7 +2755,7 @@
         </is>
       </c>
       <c r="V29" t="n">
-        <v>-0.07708244076836777</v>
+        <v>-7.708244076836777</v>
       </c>
     </row>
     <row r="30">
@@ -2835,7 +2835,7 @@
         </is>
       </c>
       <c r="V30" t="n">
-        <v>-0.01354991645079016</v>
+        <v>-1.354991645079016</v>
       </c>
     </row>
     <row r="31">
@@ -2915,7 +2915,7 @@
         </is>
       </c>
       <c r="V31" t="n">
-        <v>-0.002846718397882009</v>
+        <v>-0.2846718397882009</v>
       </c>
     </row>
     <row r="32">
@@ -2995,7 +2995,7 @@
         </is>
       </c>
       <c r="V32" t="n">
-        <v>0.00225454562032365</v>
+        <v>0.225454562032365</v>
       </c>
     </row>
     <row r="33">
@@ -3075,7 +3075,7 @@
         </is>
       </c>
       <c r="V33" t="n">
-        <v>-0.02400142801543735</v>
+        <v>-2.400142801543735</v>
       </c>
     </row>
     <row r="34">
@@ -3155,7 +3155,7 @@
         </is>
       </c>
       <c r="V34" t="n">
-        <v>-0.01350995714705207</v>
+        <v>-1.350995714705207</v>
       </c>
     </row>
     <row r="35">
@@ -3235,7 +3235,7 @@
         </is>
       </c>
       <c r="V35" t="n">
-        <v>-0.03045889830955396</v>
+        <v>-3.045889830955396</v>
       </c>
     </row>
     <row r="36">
@@ -3315,7 +3315,7 @@
         </is>
       </c>
       <c r="V36" t="n">
-        <v>-0.02986809321984917</v>
+        <v>-2.986809321984917</v>
       </c>
     </row>
     <row r="37">
@@ -3395,7 +3395,7 @@
         </is>
       </c>
       <c r="V37" t="n">
-        <v>-0.01740867144413108</v>
+        <v>-1.740867144413109</v>
       </c>
     </row>
     <row r="38">
@@ -3475,7 +3475,7 @@
         </is>
       </c>
       <c r="V38" t="n">
-        <v>0.02298358801111555</v>
+        <v>2.298358801111555</v>
       </c>
     </row>
     <row r="39">
@@ -3555,7 +3555,7 @@
         </is>
       </c>
       <c r="V39" t="n">
-        <v>-0.0421463226731227</v>
+        <v>-4.21463226731227</v>
       </c>
     </row>
     <row r="40">
@@ -3635,7 +3635,7 @@
         </is>
       </c>
       <c r="V40" t="n">
-        <v>-0.05041666001765694</v>
+        <v>-5.041666001765694</v>
       </c>
     </row>
     <row r="41">
@@ -3715,7 +3715,7 @@
         </is>
       </c>
       <c r="V41" t="n">
-        <v>-0.01228741410836448</v>
+        <v>-1.228741410836448</v>
       </c>
     </row>
     <row r="42">
@@ -3795,7 +3795,7 @@
         </is>
       </c>
       <c r="V42" t="n">
-        <v>-0.02999395400694676</v>
+        <v>-2.999395400694675</v>
       </c>
     </row>
     <row r="43">
@@ -3875,7 +3875,7 @@
         </is>
       </c>
       <c r="V43" t="n">
-        <v>-0.0468683423515194</v>
+        <v>-4.686834235151939</v>
       </c>
     </row>
     <row r="44">
@@ -3955,7 +3955,7 @@
         </is>
       </c>
       <c r="V44" t="n">
-        <v>-0.0274852132459015</v>
+        <v>-2.74852132459015</v>
       </c>
     </row>
     <row r="45">
@@ -4035,7 +4035,7 @@
         </is>
       </c>
       <c r="V45" t="n">
-        <v>-0.018006322130368</v>
+        <v>-1.8006322130368</v>
       </c>
     </row>
     <row r="46">
@@ -4115,7 +4115,7 @@
         </is>
       </c>
       <c r="V46" t="n">
-        <v>-0.03943157449362941</v>
+        <v>-3.94315744936294</v>
       </c>
     </row>
     <row r="47">
@@ -4195,7 +4195,7 @@
         </is>
       </c>
       <c r="V47" t="n">
-        <v>-0.0286441362096813</v>
+        <v>-2.864413620968131</v>
       </c>
     </row>
     <row r="48">
@@ -4275,7 +4275,7 @@
         </is>
       </c>
       <c r="V48" t="n">
-        <v>-0.01212789555846249</v>
+        <v>-1.212789555846249</v>
       </c>
     </row>
     <row r="49">
@@ -4355,7 +4355,7 @@
         </is>
       </c>
       <c r="V49" t="n">
-        <v>-0.04541812620417315</v>
+        <v>-4.541812620417315</v>
       </c>
     </row>
     <row r="50">
@@ -4435,7 +4435,7 @@
         </is>
       </c>
       <c r="V50" t="n">
-        <v>-0.03608168816305118</v>
+        <v>-3.608168816305117</v>
       </c>
     </row>
     <row r="51">
@@ -4515,7 +4515,7 @@
         </is>
       </c>
       <c r="V51" t="n">
-        <v>-0.06285360315497887</v>
+        <v>-6.285360315497887</v>
       </c>
     </row>
     <row r="52">
@@ -4595,7 +4595,7 @@
         </is>
       </c>
       <c r="V52" t="n">
-        <v>-0.04973028472009036</v>
+        <v>-4.973028472009037</v>
       </c>
     </row>
     <row r="53">
@@ -4675,7 +4675,7 @@
         </is>
       </c>
       <c r="V53" t="n">
-        <v>-0.05474915172472286</v>
+        <v>-5.474915172472286</v>
       </c>
     </row>
     <row r="54">
@@ -4755,7 +4755,7 @@
         </is>
       </c>
       <c r="V54" t="n">
-        <v>-0.00332881034127633</v>
+        <v>-0.332881034127633</v>
       </c>
     </row>
     <row r="55">
@@ -4835,7 +4835,7 @@
         </is>
       </c>
       <c r="V55" t="n">
-        <v>-0.02327162842700123</v>
+        <v>-2.327162842700123</v>
       </c>
     </row>
     <row r="56">
@@ -4915,7 +4915,7 @@
         </is>
       </c>
       <c r="V56" t="n">
-        <v>-0.02958353319528445</v>
+        <v>-2.958353319528445</v>
       </c>
     </row>
     <row r="57">
@@ -4995,7 +4995,7 @@
         </is>
       </c>
       <c r="V57" t="n">
-        <v>0.02076850573416765</v>
+        <v>2.076850573416765</v>
       </c>
     </row>
     <row r="58">
@@ -5075,7 +5075,7 @@
         </is>
       </c>
       <c r="V58" t="n">
-        <v>-0.03145322305546139</v>
+        <v>-3.145322305546139</v>
       </c>
     </row>
     <row r="59">
@@ -5155,7 +5155,7 @@
         </is>
       </c>
       <c r="V59" t="n">
-        <v>-0.007470653488961477</v>
+        <v>-0.7470653488961477</v>
       </c>
     </row>
     <row r="60">
@@ -5235,7 +5235,7 @@
         </is>
       </c>
       <c r="V60" t="n">
-        <v>0.002828487744895252</v>
+        <v>0.2828487744895252</v>
       </c>
     </row>
     <row r="61">
@@ -5315,7 +5315,7 @@
         </is>
       </c>
       <c r="V61" t="n">
-        <v>-0.002990868784666925</v>
+        <v>-0.2990868784666925</v>
       </c>
     </row>
     <row r="62">
@@ -5395,7 +5395,7 @@
         </is>
       </c>
       <c r="V62" t="n">
-        <v>-0.004256575094313014</v>
+        <v>-0.4256575094313015</v>
       </c>
     </row>
     <row r="63">
@@ -5475,7 +5475,7 @@
         </is>
       </c>
       <c r="V63" t="n">
-        <v>-0.03380060367640274</v>
+        <v>-3.380060367640275</v>
       </c>
     </row>
     <row r="64">
@@ -5555,7 +5555,7 @@
         </is>
       </c>
       <c r="V64" t="n">
-        <v>-0.01208913283707802</v>
+        <v>-1.208913283707802</v>
       </c>
     </row>
     <row r="65">
@@ -5635,7 +5635,7 @@
         </is>
       </c>
       <c r="V65" t="n">
-        <v>-0.01721516085117787</v>
+        <v>-1.721516085117788</v>
       </c>
     </row>
     <row r="66">
@@ -5715,7 +5715,7 @@
         </is>
       </c>
       <c r="V66" t="n">
-        <v>-0.0244554722484178</v>
+        <v>-2.44554722484178</v>
       </c>
     </row>
     <row r="67">
@@ -5795,7 +5795,7 @@
         </is>
       </c>
       <c r="V67" t="n">
-        <v>-0.04156891058175606</v>
+        <v>-4.156891058175606</v>
       </c>
     </row>
     <row r="68">
@@ -5875,7 +5875,7 @@
         </is>
       </c>
       <c r="V68" t="n">
-        <v>-0.02227015185260305</v>
+        <v>-2.227015185260305</v>
       </c>
     </row>
     <row r="69">
@@ -5955,7 +5955,7 @@
         </is>
       </c>
       <c r="V69" t="n">
-        <v>-0.0367929949312857</v>
+        <v>-3.679299493128569</v>
       </c>
     </row>
     <row r="70">
@@ -6035,7 +6035,7 @@
         </is>
       </c>
       <c r="V70" t="n">
-        <v>0.009813313647620255</v>
+        <v>0.9813313647620255</v>
       </c>
     </row>
     <row r="71">
@@ -6115,7 +6115,7 @@
         </is>
       </c>
       <c r="V71" t="n">
-        <v>-0.01426433068648687</v>
+        <v>-1.426433068648687</v>
       </c>
     </row>
     <row r="72">
@@ -6195,7 +6195,7 @@
         </is>
       </c>
       <c r="V72" t="n">
-        <v>-0.03276840816968993</v>
+        <v>-3.276840816968994</v>
       </c>
     </row>
     <row r="73">
@@ -6275,7 +6275,7 @@
         </is>
       </c>
       <c r="V73" t="n">
-        <v>-0.03337975198679622</v>
+        <v>-3.337975198679622</v>
       </c>
     </row>
     <row r="74">
@@ -6355,7 +6355,7 @@
         </is>
       </c>
       <c r="V74" t="n">
-        <v>-0.02632062844398159</v>
+        <v>-2.632062844398159</v>
       </c>
     </row>
     <row r="75">
@@ -6435,7 +6435,7 @@
         </is>
       </c>
       <c r="V75" t="n">
-        <v>-0.04102879391489345</v>
+        <v>-4.102879391489345</v>
       </c>
     </row>
     <row r="76">
@@ -6515,7 +6515,7 @@
         </is>
       </c>
       <c r="V76" t="n">
-        <v>-0.03615269057138866</v>
+        <v>-3.615269057138866</v>
       </c>
     </row>
     <row r="77">
@@ -6595,7 +6595,7 @@
         </is>
       </c>
       <c r="V77" t="n">
-        <v>-0.0311447190759423</v>
+        <v>-3.11447190759423</v>
       </c>
     </row>
     <row r="78">
@@ -6675,7 +6675,7 @@
         </is>
       </c>
       <c r="V78" t="n">
-        <v>-0.02111506089788784</v>
+        <v>-2.111506089788784</v>
       </c>
     </row>
     <row r="79">
@@ -6755,7 +6755,7 @@
         </is>
       </c>
       <c r="V79" t="n">
-        <v>-0.03145866745714621</v>
+        <v>-3.145866745714621</v>
       </c>
     </row>
     <row r="80">
@@ -6835,7 +6835,7 @@
         </is>
       </c>
       <c r="V80" t="n">
-        <v>-0.1014531115188736</v>
+        <v>-10.14531115188736</v>
       </c>
     </row>
     <row r="81">
@@ -6915,7 +6915,7 @@
         </is>
       </c>
       <c r="V81" t="n">
-        <v>-0.04110568386525486</v>
+        <v>-4.110568386525487</v>
       </c>
     </row>
     <row r="82">
@@ -6995,7 +6995,7 @@
         </is>
       </c>
       <c r="V82" t="n">
-        <v>-0.01374657364152947</v>
+        <v>-1.374657364152947</v>
       </c>
     </row>
     <row r="83">
@@ -7075,7 +7075,7 @@
         </is>
       </c>
       <c r="V83" t="n">
-        <v>-0.01418292510141253</v>
+        <v>-1.418292510141253</v>
       </c>
     </row>
     <row r="84">
@@ -7155,7 +7155,7 @@
         </is>
       </c>
       <c r="V84" t="n">
-        <v>-0.01471693880674202</v>
+        <v>-1.471693880674202</v>
       </c>
     </row>
     <row r="85">
@@ -7235,7 +7235,7 @@
         </is>
       </c>
       <c r="V85" t="n">
-        <v>0.004868331369381936</v>
+        <v>0.4868331369381936</v>
       </c>
     </row>
     <row r="86">
@@ -7315,7 +7315,7 @@
         </is>
       </c>
       <c r="V86" t="n">
-        <v>-0.04254629183408467</v>
+        <v>-4.254629183408467</v>
       </c>
     </row>
     <row r="87">
@@ -7395,7 +7395,7 @@
         </is>
       </c>
       <c r="V87" t="n">
-        <v>-0.02016528738371191</v>
+        <v>-2.016528738371191</v>
       </c>
     </row>
     <row r="88">
@@ -7475,7 +7475,7 @@
         </is>
       </c>
       <c r="V88" t="n">
-        <v>-0.03210717808799588</v>
+        <v>-3.210717808799588</v>
       </c>
     </row>
     <row r="89">
@@ -7555,7 +7555,7 @@
         </is>
       </c>
       <c r="V89" t="n">
-        <v>-0.05030681936292775</v>
+        <v>-5.030681936292774</v>
       </c>
     </row>
     <row r="90">
@@ -7635,7 +7635,7 @@
         </is>
       </c>
       <c r="V90" t="n">
-        <v>-0.008037628370891697</v>
+        <v>-0.8037628370891697</v>
       </c>
     </row>
     <row r="91">
@@ -7715,7 +7715,7 @@
         </is>
       </c>
       <c r="V91" t="n">
-        <v>-0.02130192011128492</v>
+        <v>-2.130192011128492</v>
       </c>
     </row>
     <row r="92">
@@ -7795,7 +7795,7 @@
         </is>
       </c>
       <c r="V92" t="n">
-        <v>-0.01108513356388517</v>
+        <v>-1.108513356388517</v>
       </c>
     </row>
     <row r="93">
@@ -7875,7 +7875,7 @@
         </is>
       </c>
       <c r="V93" t="n">
-        <v>-0.03907611830891281</v>
+        <v>-3.907611830891281</v>
       </c>
     </row>
     <row r="94">
@@ -7955,7 +7955,7 @@
         </is>
       </c>
       <c r="V94" t="n">
-        <v>-0.04118019672572016</v>
+        <v>-4.118019672572016</v>
       </c>
     </row>
     <row r="95">
@@ -8035,7 +8035,7 @@
         </is>
       </c>
       <c r="V95" t="n">
-        <v>0.1148996346141485</v>
+        <v>11.48996346141485</v>
       </c>
     </row>
     <row r="96">
@@ -8115,7 +8115,7 @@
         </is>
       </c>
       <c r="V96" t="n">
-        <v>-0.0287515697748225</v>
+        <v>-2.87515697748225</v>
       </c>
     </row>
     <row r="97">
@@ -8195,7 +8195,7 @@
         </is>
       </c>
       <c r="V97" t="n">
-        <v>-0.02522742820392277</v>
+        <v>-2.522742820392277</v>
       </c>
     </row>
     <row r="98">
@@ -8275,7 +8275,7 @@
         </is>
       </c>
       <c r="V98" t="n">
-        <v>-0.01857507519234883</v>
+        <v>-1.857507519234883</v>
       </c>
     </row>
     <row r="99">
@@ -8355,7 +8355,7 @@
         </is>
       </c>
       <c r="V99" t="n">
-        <v>-0.03103461539061256</v>
+        <v>-3.103461539061256</v>
       </c>
     </row>
     <row r="100">
@@ -8435,7 +8435,7 @@
         </is>
       </c>
       <c r="V100" t="n">
-        <v>-0.005733871366737643</v>
+        <v>-0.5733871366737643</v>
       </c>
     </row>
     <row r="101">
@@ -8515,7 +8515,7 @@
         </is>
       </c>
       <c r="V101" t="n">
-        <v>-0.03585364809220387</v>
+        <v>-3.585364809220387</v>
       </c>
     </row>
     <row r="102">
@@ -8595,7 +8595,7 @@
         </is>
       </c>
       <c r="V102" t="n">
-        <v>0.00422125687756205</v>
+        <v>0.422125687756205</v>
       </c>
     </row>
     <row r="103">
@@ -8675,7 +8675,7 @@
         </is>
       </c>
       <c r="V103" t="n">
-        <v>-0.02363863138643421</v>
+        <v>-2.363863138643421</v>
       </c>
     </row>
     <row r="104">
@@ -8755,7 +8755,7 @@
         </is>
       </c>
       <c r="V104" t="n">
-        <v>-0.03028610367101815</v>
+        <v>-3.028610367101816</v>
       </c>
     </row>
     <row r="105">
@@ -8835,7 +8835,7 @@
         </is>
       </c>
       <c r="V105" t="n">
-        <v>-0.01668535266178965</v>
+        <v>-1.668535266178965</v>
       </c>
     </row>
     <row r="106">
@@ -8915,7 +8915,7 @@
         </is>
       </c>
       <c r="V106" t="n">
-        <v>-0.03440699875481342</v>
+        <v>-3.440699875481342</v>
       </c>
     </row>
     <row r="107">
@@ -8995,7 +8995,7 @@
         </is>
       </c>
       <c r="V107" t="n">
-        <v>-0.03405073736539824</v>
+        <v>-3.405073736539824</v>
       </c>
     </row>
     <row r="108">
@@ -9075,7 +9075,7 @@
         </is>
       </c>
       <c r="V108" t="n">
-        <v>-0.06443699806862473</v>
+        <v>-6.443699806862473</v>
       </c>
     </row>
     <row r="109">
@@ -9155,7 +9155,7 @@
         </is>
       </c>
       <c r="V109" t="n">
-        <v>0.002305479351703594</v>
+        <v>0.2305479351703593</v>
       </c>
     </row>
     <row r="110">
@@ -9235,7 +9235,7 @@
         </is>
       </c>
       <c r="V110" t="n">
-        <v>-0.02521882051041456</v>
+        <v>-2.521882051041456</v>
       </c>
     </row>
     <row r="111">
@@ -9315,7 +9315,7 @@
         </is>
       </c>
       <c r="V111" t="n">
-        <v>-0.01848249590153418</v>
+        <v>-1.848249590153418</v>
       </c>
     </row>
     <row r="112">
@@ -9395,7 +9395,7 @@
         </is>
       </c>
       <c r="V112" t="n">
-        <v>-0.0177916276418841</v>
+        <v>-1.77916276418841</v>
       </c>
     </row>
     <row r="113">
@@ -9475,7 +9475,7 @@
         </is>
       </c>
       <c r="V113" t="n">
-        <v>-0.02712950512199258</v>
+        <v>-2.712950512199258</v>
       </c>
     </row>
     <row r="114">
@@ -9555,7 +9555,7 @@
         </is>
       </c>
       <c r="V114" t="n">
-        <v>-0.01868945577905195</v>
+        <v>-1.868945577905195</v>
       </c>
     </row>
     <row r="115">
@@ -9635,7 +9635,7 @@
         </is>
       </c>
       <c r="V115" t="n">
-        <v>-0.04442915307396002</v>
+        <v>-4.442915307396002</v>
       </c>
     </row>
     <row r="116">
@@ -9715,7 +9715,7 @@
         </is>
       </c>
       <c r="V116" t="n">
-        <v>-0.009288361236154856</v>
+        <v>-0.9288361236154857</v>
       </c>
     </row>
     <row r="117">
@@ -9795,7 +9795,7 @@
         </is>
       </c>
       <c r="V117" t="n">
-        <v>-0.03148634275252381</v>
+        <v>-3.148634275252381</v>
       </c>
     </row>
     <row r="118">
@@ -9875,7 +9875,7 @@
         </is>
       </c>
       <c r="V118" t="n">
-        <v>-0.0210608140685666</v>
+        <v>-2.10608140685666</v>
       </c>
     </row>
     <row r="119">
@@ -9955,7 +9955,7 @@
         </is>
       </c>
       <c r="V119" t="n">
-        <v>-0.03742913095904383</v>
+        <v>-3.742913095904383</v>
       </c>
     </row>
     <row r="120">
@@ -10035,7 +10035,7 @@
         </is>
       </c>
       <c r="V120" t="n">
-        <v>-0.04606428745614561</v>
+        <v>-4.606428745614561</v>
       </c>
     </row>
     <row r="121">
@@ -10115,7 +10115,7 @@
         </is>
       </c>
       <c r="V121" t="n">
-        <v>-0.03019107506715167</v>
+        <v>-3.019107506715166</v>
       </c>
     </row>
     <row r="122">
@@ -10195,7 +10195,7 @@
         </is>
       </c>
       <c r="V122" t="n">
-        <v>0.03599976466170274</v>
+        <v>3.599976466170274</v>
       </c>
     </row>
     <row r="123">
@@ -10275,7 +10275,7 @@
         </is>
       </c>
       <c r="V123" t="n">
-        <v>-0.02784243261187225</v>
+        <v>-2.784243261187225</v>
       </c>
     </row>
     <row r="124">
@@ -10355,7 +10355,7 @@
         </is>
       </c>
       <c r="V124" t="n">
-        <v>-0.003230681739759642</v>
+        <v>-0.3230681739759642</v>
       </c>
     </row>
     <row r="125">
@@ -10435,7 +10435,7 @@
         </is>
       </c>
       <c r="V125" t="n">
-        <v>-0.01086784161136056</v>
+        <v>-1.086784161136056</v>
       </c>
     </row>
     <row r="126">
@@ -10515,7 +10515,7 @@
         </is>
       </c>
       <c r="V126" t="n">
-        <v>-0.006990999729136958</v>
+        <v>-0.6990999729136957</v>
       </c>
     </row>
     <row r="127">
@@ -10595,7 +10595,7 @@
         </is>
       </c>
       <c r="V127" t="n">
-        <v>-0.03395600549502172</v>
+        <v>-3.395600549502172</v>
       </c>
     </row>
     <row r="128">
@@ -10675,7 +10675,7 @@
         </is>
       </c>
       <c r="V128" t="n">
-        <v>-0.05406403533281193</v>
+        <v>-5.406403533281193</v>
       </c>
     </row>
     <row r="129">
@@ -10755,7 +10755,7 @@
         </is>
       </c>
       <c r="V129" t="n">
-        <v>-0.05759797618256795</v>
+        <v>-5.759797618256795</v>
       </c>
     </row>
     <row r="130">
@@ -10835,7 +10835,7 @@
         </is>
       </c>
       <c r="V130" t="n">
-        <v>-0.0309762647083019</v>
+        <v>-3.09762647083019</v>
       </c>
     </row>
     <row r="131">
@@ -10915,7 +10915,7 @@
         </is>
       </c>
       <c r="V131" t="n">
-        <v>-0.06931295608440081</v>
+        <v>-6.931295608440082</v>
       </c>
     </row>
     <row r="132">
@@ -10995,7 +10995,7 @@
         </is>
       </c>
       <c r="V132" t="n">
-        <v>0.04552326517363181</v>
+        <v>4.552326517363182</v>
       </c>
     </row>
     <row r="133">
@@ -11075,7 +11075,7 @@
         </is>
       </c>
       <c r="V133" t="n">
-        <v>-0.04502774001772303</v>
+        <v>-4.502774001772303</v>
       </c>
     </row>
     <row r="134">
@@ -11155,7 +11155,7 @@
         </is>
       </c>
       <c r="V134" t="n">
-        <v>-0.02734785362508843</v>
+        <v>-2.734785362508843</v>
       </c>
     </row>
     <row r="135">
@@ -11235,7 +11235,7 @@
         </is>
       </c>
       <c r="V135" t="n">
-        <v>0.01898382752412984</v>
+        <v>1.898382752412984</v>
       </c>
     </row>
     <row r="136">
@@ -11315,7 +11315,7 @@
         </is>
       </c>
       <c r="V136" t="n">
-        <v>-0.06899481889017173</v>
+        <v>-6.899481889017173</v>
       </c>
     </row>
     <row r="137">
@@ -11395,7 +11395,7 @@
         </is>
       </c>
       <c r="V137" t="n">
-        <v>-0.04310070850655964</v>
+        <v>-4.310070850655964</v>
       </c>
     </row>
     <row r="138">
@@ -11475,7 +11475,7 @@
         </is>
       </c>
       <c r="V138" t="n">
-        <v>-0.0164586810145942</v>
+        <v>-1.64586810145942</v>
       </c>
     </row>
     <row r="139">
@@ -11555,7 +11555,7 @@
         </is>
       </c>
       <c r="V139" t="n">
-        <v>-0.02764640954505996</v>
+        <v>-2.764640954505996</v>
       </c>
     </row>
     <row r="140">
@@ -11635,7 +11635,7 @@
         </is>
       </c>
       <c r="V140" t="n">
-        <v>-0.02534981451406505</v>
+        <v>-2.534981451406505</v>
       </c>
     </row>
     <row r="141">
@@ -11715,7 +11715,7 @@
         </is>
       </c>
       <c r="V141" t="n">
-        <v>-0.02657942111156249</v>
+        <v>-2.657942111156249</v>
       </c>
     </row>
     <row r="142">
@@ -11795,7 +11795,7 @@
         </is>
       </c>
       <c r="V142" t="n">
-        <v>-0.02986450045122585</v>
+        <v>-2.986450045122584</v>
       </c>
     </row>
     <row r="143">
@@ -11875,7 +11875,7 @@
         </is>
       </c>
       <c r="V143" t="n">
-        <v>-0.02818304617776572</v>
+        <v>-2.818304617776572</v>
       </c>
     </row>
     <row r="144">
@@ -11955,7 +11955,7 @@
         </is>
       </c>
       <c r="V144" t="n">
-        <v>-0.03528169608249762</v>
+        <v>-3.528169608249762</v>
       </c>
     </row>
     <row r="145">
@@ -12035,7 +12035,7 @@
         </is>
       </c>
       <c r="V145" t="n">
-        <v>-0.03659748489437211</v>
+        <v>-3.659748489437211</v>
       </c>
     </row>
     <row r="146">
@@ -12115,7 +12115,7 @@
         </is>
       </c>
       <c r="V146" t="n">
-        <v>-0.02060444643347544</v>
+        <v>-2.060444643347544</v>
       </c>
     </row>
     <row r="147">
@@ -12195,7 +12195,7 @@
         </is>
       </c>
       <c r="V147" t="n">
-        <v>0.03145420963154026</v>
+        <v>3.145420963154026</v>
       </c>
     </row>
     <row r="148">
@@ -12275,7 +12275,7 @@
         </is>
       </c>
       <c r="V148" t="n">
-        <v>-0.04501834533211457</v>
+        <v>-4.501834533211457</v>
       </c>
     </row>
     <row r="149">
@@ -12355,7 +12355,7 @@
         </is>
       </c>
       <c r="V149" t="n">
-        <v>-0.03083488915064071</v>
+        <v>-3.083488915064071</v>
       </c>
     </row>
     <row r="150">
@@ -12435,7 +12435,7 @@
         </is>
       </c>
       <c r="V150" t="n">
-        <v>-0.03659171907563687</v>
+        <v>-3.659171907563687</v>
       </c>
     </row>
     <row r="151">
@@ -12515,7 +12515,7 @@
         </is>
       </c>
       <c r="V151" t="n">
-        <v>0.00214792330784494</v>
+        <v>0.214792330784494</v>
       </c>
     </row>
     <row r="152">
@@ -12595,7 +12595,7 @@
         </is>
       </c>
       <c r="V152" t="n">
-        <v>-0.01997278961361583</v>
+        <v>-1.997278961361583</v>
       </c>
     </row>
     <row r="153">
@@ -12675,7 +12675,7 @@
         </is>
       </c>
       <c r="V153" t="n">
-        <v>-0.04139151439220543</v>
+        <v>-4.139151439220544</v>
       </c>
     </row>
     <row r="154">
@@ -12755,7 +12755,7 @@
         </is>
       </c>
       <c r="V154" t="n">
-        <v>-0.04341970438623122</v>
+        <v>-4.341970438623122</v>
       </c>
     </row>
     <row r="155">
@@ -12835,7 +12835,7 @@
         </is>
       </c>
       <c r="V155" t="n">
-        <v>-0.04020381496905393</v>
+        <v>-4.020381496905394</v>
       </c>
     </row>
     <row r="156">
@@ -12915,7 +12915,7 @@
         </is>
       </c>
       <c r="V156" t="n">
-        <v>-0.008945756862743416</v>
+        <v>-0.8945756862743416</v>
       </c>
     </row>
     <row r="157">
@@ -12995,7 +12995,7 @@
         </is>
       </c>
       <c r="V157" t="n">
-        <v>-0.008233307650047372</v>
+        <v>-0.8233307650047372</v>
       </c>
     </row>
     <row r="158">
@@ -13075,7 +13075,7 @@
         </is>
       </c>
       <c r="V158" t="n">
-        <v>-0.02455567627195859</v>
+        <v>-2.45556762719586</v>
       </c>
     </row>
     <row r="159">
@@ -13155,7 +13155,7 @@
         </is>
       </c>
       <c r="V159" t="n">
-        <v>-0.05351724292924414</v>
+        <v>-5.351724292924414</v>
       </c>
     </row>
     <row r="160">
@@ -13235,7 +13235,7 @@
         </is>
       </c>
       <c r="V160" t="n">
-        <v>0.02847113011932829</v>
+        <v>2.847113011932829</v>
       </c>
     </row>
     <row r="161">
@@ -13315,7 +13315,7 @@
         </is>
       </c>
       <c r="V161" t="n">
-        <v>-0.02255101327389643</v>
+        <v>-2.255101327389643</v>
       </c>
     </row>
     <row r="162">
@@ -13395,7 +13395,7 @@
         </is>
       </c>
       <c r="V162" t="n">
-        <v>-0.01908561809193959</v>
+        <v>-1.908561809193959</v>
       </c>
     </row>
     <row r="163">
@@ -13475,7 +13475,7 @@
         </is>
       </c>
       <c r="V163" t="n">
-        <v>-0.02743682577517599</v>
+        <v>-2.743682577517598</v>
       </c>
     </row>
     <row r="164">
@@ -13555,7 +13555,7 @@
         </is>
       </c>
       <c r="V164" t="n">
-        <v>-0.0229931779358363</v>
+        <v>-2.29931779358363</v>
       </c>
     </row>
     <row r="165">
@@ -13635,7 +13635,7 @@
         </is>
       </c>
       <c r="V165" t="n">
-        <v>-0.06407084894383386</v>
+        <v>-6.407084894383385</v>
       </c>
     </row>
     <row r="166">
@@ -13715,7 +13715,7 @@
         </is>
       </c>
       <c r="V166" t="n">
-        <v>-0.02622716034918423</v>
+        <v>-2.622716034918423</v>
       </c>
     </row>
     <row r="167">
@@ -13795,7 +13795,7 @@
         </is>
       </c>
       <c r="V167" t="n">
-        <v>-0.03648619853180068</v>
+        <v>-3.648619853180068</v>
       </c>
     </row>
     <row r="168">
@@ -13875,7 +13875,7 @@
         </is>
       </c>
       <c r="V168" t="n">
-        <v>-0.00988979869153927</v>
+        <v>-0.988979869153927</v>
       </c>
     </row>
     <row r="169">
@@ -13955,7 +13955,7 @@
         </is>
       </c>
       <c r="V169" t="n">
-        <v>-0.01644216949653326</v>
+        <v>-1.644216949653326</v>
       </c>
     </row>
     <row r="170">
@@ -14035,7 +14035,7 @@
         </is>
       </c>
       <c r="V170" t="n">
-        <v>-0.03244108112499367</v>
+        <v>-3.244108112499367</v>
       </c>
     </row>
     <row r="171">
@@ -14115,7 +14115,7 @@
         </is>
       </c>
       <c r="V171" t="n">
-        <v>-0.04617461034197268</v>
+        <v>-4.617461034197268</v>
       </c>
     </row>
     <row r="172">
@@ -14195,7 +14195,7 @@
         </is>
       </c>
       <c r="V172" t="n">
-        <v>-0.01907883843746446</v>
+        <v>-1.907883843746446</v>
       </c>
     </row>
     <row r="173">
@@ -14275,7 +14275,7 @@
         </is>
       </c>
       <c r="V173" t="n">
-        <v>0.1118926792608279</v>
+        <v>11.18926792608279</v>
       </c>
     </row>
     <row r="174">
@@ -14355,7 +14355,7 @@
         </is>
       </c>
       <c r="V174" t="n">
-        <v>-0.02596958651195092</v>
+        <v>-2.596958651195092</v>
       </c>
     </row>
     <row r="175">
@@ -14435,7 +14435,7 @@
         </is>
       </c>
       <c r="V175" t="n">
-        <v>-0.005113169489411464</v>
+        <v>-0.5113169489411464</v>
       </c>
     </row>
     <row r="176">
@@ -14515,7 +14515,7 @@
         </is>
       </c>
       <c r="V176" t="n">
-        <v>-0.008832141837422888</v>
+        <v>-0.8832141837422888</v>
       </c>
     </row>
     <row r="177">
@@ -14595,7 +14595,7 @@
         </is>
       </c>
       <c r="V177" t="n">
-        <v>-0.05659778036841038</v>
+        <v>-5.659778036841039</v>
       </c>
     </row>
     <row r="178">
@@ -14675,7 +14675,7 @@
         </is>
       </c>
       <c r="V178" t="n">
-        <v>-0.02387101399806946</v>
+        <v>-2.387101399806946</v>
       </c>
     </row>
     <row r="179">
@@ -14755,7 +14755,7 @@
         </is>
       </c>
       <c r="V179" t="n">
-        <v>-0.04308449639964562</v>
+        <v>-4.308449639964562</v>
       </c>
     </row>
     <row r="180">
@@ -14835,7 +14835,7 @@
         </is>
       </c>
       <c r="V180" t="n">
-        <v>-0.004188316060556319</v>
+        <v>-0.4188316060556319</v>
       </c>
     </row>
     <row r="181">
@@ -14915,7 +14915,7 @@
         </is>
       </c>
       <c r="V181" t="n">
-        <v>-0.02940027546334526</v>
+        <v>-2.940027546334527</v>
       </c>
     </row>
     <row r="182">
@@ -14995,7 +14995,7 @@
         </is>
       </c>
       <c r="V182" t="n">
-        <v>-0.02111887944172099</v>
+        <v>-2.111887944172099</v>
       </c>
     </row>
     <row r="183">
@@ -15075,7 +15075,7 @@
         </is>
       </c>
       <c r="V183" t="n">
-        <v>-0.04165154368141493</v>
+        <v>-4.165154368141493</v>
       </c>
     </row>
     <row r="184">
@@ -15155,7 +15155,7 @@
         </is>
       </c>
       <c r="V184" t="n">
-        <v>-0.01828254858595958</v>
+        <v>-1.828254858595957</v>
       </c>
     </row>
     <row r="185">
@@ -15235,7 +15235,7 @@
         </is>
       </c>
       <c r="V185" t="n">
-        <v>-0.02647734803830993</v>
+        <v>-2.647734803830993</v>
       </c>
     </row>
     <row r="186">
@@ -15315,7 +15315,7 @@
         </is>
       </c>
       <c r="V186" t="n">
-        <v>-0.0246755438341988</v>
+        <v>-2.467554383419881</v>
       </c>
     </row>
     <row r="187">
@@ -15395,7 +15395,7 @@
         </is>
       </c>
       <c r="V187" t="n">
-        <v>-0.02882064826829041</v>
+        <v>-2.882064826829041</v>
       </c>
     </row>
     <row r="188">
@@ -15475,7 +15475,7 @@
         </is>
       </c>
       <c r="V188" t="n">
-        <v>-0.009877386765881086</v>
+        <v>-0.9877386765881085</v>
       </c>
     </row>
     <row r="189">
@@ -15555,7 +15555,7 @@
         </is>
       </c>
       <c r="V189" t="n">
-        <v>-0.03531454518845444</v>
+        <v>-3.531454518845444</v>
       </c>
     </row>
     <row r="190">
@@ -15635,7 +15635,7 @@
         </is>
       </c>
       <c r="V190" t="n">
-        <v>-0.02542950725723505</v>
+        <v>-2.542950725723505</v>
       </c>
     </row>
     <row r="191">
@@ -15715,7 +15715,7 @@
         </is>
       </c>
       <c r="V191" t="n">
-        <v>0.003600615966581233</v>
+        <v>0.3600615966581233</v>
       </c>
     </row>
     <row r="192">
@@ -15795,7 +15795,7 @@
         </is>
       </c>
       <c r="V192" t="n">
-        <v>-0.001457525553647347</v>
+        <v>-0.1457525553647347</v>
       </c>
     </row>
     <row r="193">
@@ -15875,7 +15875,7 @@
         </is>
       </c>
       <c r="V193" t="n">
-        <v>-0.05481807858931986</v>
+        <v>-5.481807858931987</v>
       </c>
     </row>
     <row r="194">
@@ -15955,7 +15955,7 @@
         </is>
       </c>
       <c r="V194" t="n">
-        <v>-0.06410257178274333</v>
+        <v>-6.410257178274332</v>
       </c>
     </row>
     <row r="195">
@@ -16035,7 +16035,7 @@
         </is>
       </c>
       <c r="V195" t="n">
-        <v>-0.05362065812309443</v>
+        <v>-5.362065812309443</v>
       </c>
     </row>
     <row r="196">
@@ -16115,7 +16115,7 @@
         </is>
       </c>
       <c r="V196" t="n">
-        <v>0.0193206181940537</v>
+        <v>1.93206181940537</v>
       </c>
     </row>
     <row r="197">
@@ -16195,7 +16195,7 @@
         </is>
       </c>
       <c r="V197" t="n">
-        <v>-0.01238172539548517</v>
+        <v>-1.238172539548517</v>
       </c>
     </row>
     <row r="198">
@@ -16275,7 +16275,7 @@
         </is>
       </c>
       <c r="V198" t="n">
-        <v>-0.02852536575209957</v>
+        <v>-2.852536575209957</v>
       </c>
     </row>
     <row r="199">
@@ -16355,7 +16355,7 @@
         </is>
       </c>
       <c r="V199" t="n">
-        <v>0.06106510925101933</v>
+        <v>6.106510925101933</v>
       </c>
     </row>
     <row r="200">
@@ -16435,7 +16435,7 @@
         </is>
       </c>
       <c r="V200" t="n">
-        <v>-0.08662455617140125</v>
+        <v>-8.662455617140123</v>
       </c>
     </row>
     <row r="201">
@@ -16515,7 +16515,7 @@
         </is>
       </c>
       <c r="V201" t="n">
-        <v>-0.008705464509657984</v>
+        <v>-0.8705464509657984</v>
       </c>
     </row>
     <row r="202">
@@ -16595,7 +16595,7 @@
         </is>
       </c>
       <c r="V202" t="n">
-        <v>-0.01311758704299844</v>
+        <v>-1.311758704299844</v>
       </c>
     </row>
     <row r="203">
@@ -16675,7 +16675,7 @@
         </is>
       </c>
       <c r="V203" t="n">
-        <v>-0.01955144619666009</v>
+        <v>-1.955144619666009</v>
       </c>
     </row>
     <row r="204">
@@ -16755,7 +16755,7 @@
         </is>
       </c>
       <c r="V204" t="n">
-        <v>0.01465579921917403</v>
+        <v>1.465579921917403</v>
       </c>
     </row>
     <row r="205">
@@ -16835,7 +16835,7 @@
         </is>
       </c>
       <c r="V205" t="n">
-        <v>-0.06380512028296802</v>
+        <v>-6.380512028296803</v>
       </c>
     </row>
     <row r="206">
@@ -16915,7 +16915,7 @@
         </is>
       </c>
       <c r="V206" t="n">
-        <v>-0.02216617784703468</v>
+        <v>-2.216617784703468</v>
       </c>
     </row>
     <row r="207">
@@ -16995,7 +16995,7 @@
         </is>
       </c>
       <c r="V207" t="n">
-        <v>-0.01742941373164737</v>
+        <v>-1.742941373164737</v>
       </c>
     </row>
     <row r="208">
@@ -17075,7 +17075,7 @@
         </is>
       </c>
       <c r="V208" t="n">
-        <v>-0.03877674236397451</v>
+        <v>-3.877674236397452</v>
       </c>
     </row>
     <row r="209">
@@ -17155,7 +17155,7 @@
         </is>
       </c>
       <c r="V209" t="n">
-        <v>-0.06983358291800799</v>
+        <v>-6.9833582918008</v>
       </c>
     </row>
     <row r="210">
@@ -17235,7 +17235,7 @@
         </is>
       </c>
       <c r="V210" t="n">
-        <v>-0.03242101274100132</v>
+        <v>-3.242101274100132</v>
       </c>
     </row>
     <row r="211">
@@ -17315,7 +17315,7 @@
         </is>
       </c>
       <c r="V211" t="n">
-        <v>-0.02262992416906051</v>
+        <v>-2.262992416906051</v>
       </c>
     </row>
     <row r="212">
@@ -17395,7 +17395,7 @@
         </is>
       </c>
       <c r="V212" t="n">
-        <v>-0.01657514977219367</v>
+        <v>-1.657514977219367</v>
       </c>
     </row>
     <row r="213">
@@ -17475,7 +17475,7 @@
         </is>
       </c>
       <c r="V213" t="n">
-        <v>-0.00397576167462798</v>
+        <v>-0.397576167462798</v>
       </c>
     </row>
     <row r="214">
@@ -17555,7 +17555,7 @@
         </is>
       </c>
       <c r="V214" t="n">
-        <v>-0.03755086965429687</v>
+        <v>-3.755086965429687</v>
       </c>
     </row>
     <row r="215">
@@ -17635,7 +17635,7 @@
         </is>
       </c>
       <c r="V215" t="n">
-        <v>-0.03308927779590858</v>
+        <v>-3.308927779590858</v>
       </c>
     </row>
     <row r="216">
@@ -17715,7 +17715,7 @@
         </is>
       </c>
       <c r="V216" t="n">
-        <v>-0.0537078135285147</v>
+        <v>-5.37078135285147</v>
       </c>
     </row>
     <row r="217">
@@ -17795,7 +17795,7 @@
         </is>
       </c>
       <c r="V217" t="n">
-        <v>-0.04437556516985292</v>
+        <v>-4.437556516985292</v>
       </c>
     </row>
     <row r="218">
@@ -17875,7 +17875,7 @@
         </is>
       </c>
       <c r="V218" t="n">
-        <v>0.0102601194398276</v>
+        <v>1.02601194398276</v>
       </c>
     </row>
     <row r="219">
@@ -17955,7 +17955,7 @@
         </is>
       </c>
       <c r="V219" t="n">
-        <v>-0.03770552319960783</v>
+        <v>-3.770552319960782</v>
       </c>
     </row>
     <row r="220">
@@ -18035,7 +18035,7 @@
         </is>
       </c>
       <c r="V220" t="n">
-        <v>-0.007715658424359474</v>
+        <v>-0.7715658424359474</v>
       </c>
     </row>
     <row r="221">
@@ -18115,7 +18115,7 @@
         </is>
       </c>
       <c r="V221" t="n">
-        <v>-0.04082394645896859</v>
+        <v>-4.082394645896859</v>
       </c>
     </row>
     <row r="222">
@@ -18195,7 +18195,7 @@
         </is>
       </c>
       <c r="V222" t="n">
-        <v>0.01114135110854774</v>
+        <v>1.114135110854774</v>
       </c>
     </row>
     <row r="223">
@@ -18275,7 +18275,7 @@
         </is>
       </c>
       <c r="V223" t="n">
-        <v>-0.03960994453303025</v>
+        <v>-3.960994453303025</v>
       </c>
     </row>
     <row r="224">
@@ -18355,7 +18355,7 @@
         </is>
       </c>
       <c r="V224" t="n">
-        <v>0.03092846821605257</v>
+        <v>3.092846821605256</v>
       </c>
     </row>
     <row r="225">
@@ -18435,7 +18435,7 @@
         </is>
       </c>
       <c r="V225" t="n">
-        <v>-0.03516526901577017</v>
+        <v>-3.516526901577016</v>
       </c>
     </row>
     <row r="226">
@@ -18515,7 +18515,7 @@
         </is>
       </c>
       <c r="V226" t="n">
-        <v>-0.0275073212755053</v>
+        <v>-2.75073212755053</v>
       </c>
     </row>
     <row r="227">
@@ -18595,7 +18595,7 @@
         </is>
       </c>
       <c r="V227" t="n">
-        <v>-0.04200547094832707</v>
+        <v>-4.200547094832707</v>
       </c>
     </row>
     <row r="228">
@@ -18675,7 +18675,7 @@
         </is>
       </c>
       <c r="V228" t="n">
-        <v>-0.04044521328253161</v>
+        <v>-4.044521328253161</v>
       </c>
     </row>
     <row r="229">
@@ -18755,7 +18755,7 @@
         </is>
       </c>
       <c r="V229" t="n">
-        <v>-0.02188728288911957</v>
+        <v>-2.188728288911957</v>
       </c>
     </row>
     <row r="230">
@@ -18835,7 +18835,7 @@
         </is>
       </c>
       <c r="V230" t="n">
-        <v>-0.01276482806421362</v>
+        <v>-1.276482806421362</v>
       </c>
     </row>
     <row r="231">
@@ -18915,7 +18915,7 @@
         </is>
       </c>
       <c r="V231" t="n">
-        <v>-0.01128616310984422</v>
+        <v>-1.128616310984422</v>
       </c>
     </row>
     <row r="232">
@@ -18995,7 +18995,7 @@
         </is>
       </c>
       <c r="V232" t="n">
-        <v>-0.0287234780588656</v>
+        <v>-2.872347805886561</v>
       </c>
     </row>
     <row r="233">
@@ -19075,7 +19075,7 @@
         </is>
       </c>
       <c r="V233" t="n">
-        <v>-0.03517807227469038</v>
+        <v>-3.517807227469037</v>
       </c>
     </row>
     <row r="234">
@@ -19155,7 +19155,7 @@
         </is>
       </c>
       <c r="V234" t="n">
-        <v>-0.0295678335329096</v>
+        <v>-2.95678335329096</v>
       </c>
     </row>
     <row r="235">
@@ -19235,7 +19235,7 @@
         </is>
       </c>
       <c r="V235" t="n">
-        <v>-0.05316400082564488</v>
+        <v>-5.316400082564488</v>
       </c>
     </row>
     <row r="236">
@@ -19315,7 +19315,7 @@
         </is>
       </c>
       <c r="V236" t="n">
-        <v>-0.02752670743566825</v>
+        <v>-2.752670743566824</v>
       </c>
     </row>
     <row r="237">
@@ -19395,7 +19395,7 @@
         </is>
       </c>
       <c r="V237" t="n">
-        <v>-0.02839830316077111</v>
+        <v>-2.839830316077111</v>
       </c>
     </row>
     <row r="238">
@@ -19475,7 +19475,7 @@
         </is>
       </c>
       <c r="V238" t="n">
-        <v>0.01609188320772943</v>
+        <v>1.609188320772943</v>
       </c>
     </row>
     <row r="239">
@@ -19555,7 +19555,7 @@
         </is>
       </c>
       <c r="V239" t="n">
-        <v>-0.00304053255929935</v>
+        <v>-0.304053255929935</v>
       </c>
     </row>
     <row r="240">
@@ -19635,7 +19635,7 @@
         </is>
       </c>
       <c r="V240" t="n">
-        <v>-0.02751475724983871</v>
+        <v>-2.751475724983871</v>
       </c>
     </row>
     <row r="241">
@@ -19715,7 +19715,7 @@
         </is>
       </c>
       <c r="V241" t="n">
-        <v>-0.03055293108791476</v>
+        <v>-3.055293108791476</v>
       </c>
     </row>
     <row r="242">
@@ -19795,7 +19795,7 @@
         </is>
       </c>
       <c r="V242" t="n">
-        <v>0.1994632120973422</v>
+        <v>19.94632120973422</v>
       </c>
     </row>
     <row r="243">
@@ -19875,7 +19875,7 @@
         </is>
       </c>
       <c r="V243" t="n">
-        <v>-0.04663369930193437</v>
+        <v>-4.663369930193437</v>
       </c>
     </row>
     <row r="244">
@@ -19955,7 +19955,7 @@
         </is>
       </c>
       <c r="V244" t="n">
-        <v>-0.03063391776119758</v>
+        <v>-3.063391776119758</v>
       </c>
     </row>
     <row r="245">
@@ -20035,7 +20035,7 @@
         </is>
       </c>
       <c r="V245" t="n">
-        <v>-0.07344368409280973</v>
+        <v>-7.344368409280972</v>
       </c>
     </row>
     <row r="246">
@@ -20115,7 +20115,7 @@
         </is>
       </c>
       <c r="V246" t="n">
-        <v>-0.02386249326864197</v>
+        <v>-2.386249326864197</v>
       </c>
     </row>
     <row r="247">
@@ -20195,7 +20195,7 @@
         </is>
       </c>
       <c r="V247" t="n">
-        <v>-0.03812186413146574</v>
+        <v>-3.812186413146573</v>
       </c>
     </row>
     <row r="248">
@@ -20275,7 +20275,7 @@
         </is>
       </c>
       <c r="V248" t="n">
-        <v>-0.009889667041823584</v>
+        <v>-0.9889667041823583</v>
       </c>
     </row>
     <row r="249">
@@ -20355,7 +20355,7 @@
         </is>
       </c>
       <c r="V249" t="n">
-        <v>-0.05247805136896818</v>
+        <v>-5.247805136896818</v>
       </c>
     </row>
     <row r="250">
@@ -20435,7 +20435,7 @@
         </is>
       </c>
       <c r="V250" t="n">
-        <v>-0.0266143701468392</v>
+        <v>-2.66143701468392</v>
       </c>
     </row>
     <row r="251">
@@ -20515,7 +20515,7 @@
         </is>
       </c>
       <c r="V251" t="n">
-        <v>-0.01169500965710967</v>
+        <v>-1.169500965710967</v>
       </c>
     </row>
     <row r="252">
@@ -20595,7 +20595,7 @@
         </is>
       </c>
       <c r="V252" t="n">
-        <v>0.004192612818547568</v>
+        <v>0.4192612818547568</v>
       </c>
     </row>
     <row r="253">
@@ -20675,7 +20675,7 @@
         </is>
       </c>
       <c r="V253" t="n">
-        <v>-0.01920944666267459</v>
+        <v>-1.920944666267459</v>
       </c>
     </row>
     <row r="254">
@@ -20755,7 +20755,7 @@
         </is>
       </c>
       <c r="V254" t="n">
-        <v>-0.04396210375727544</v>
+        <v>-4.396210375727544</v>
       </c>
     </row>
     <row r="255">
@@ -20835,7 +20835,7 @@
         </is>
       </c>
       <c r="V255" t="n">
-        <v>-0.02359996107963849</v>
+        <v>-2.359996107963849</v>
       </c>
     </row>
     <row r="256">
@@ -20915,7 +20915,7 @@
         </is>
       </c>
       <c r="V256" t="n">
-        <v>-0.03079883747949573</v>
+        <v>-3.079883747949574</v>
       </c>
     </row>
     <row r="257">
@@ -20995,7 +20995,7 @@
         </is>
       </c>
       <c r="V257" t="n">
-        <v>-0.01767788667965128</v>
+        <v>-1.767788667965128</v>
       </c>
     </row>
     <row r="258">
@@ -21075,7 +21075,7 @@
         </is>
       </c>
       <c r="V258" t="n">
-        <v>-0.02988565522958402</v>
+        <v>-2.988565522958401</v>
       </c>
     </row>
     <row r="259">
@@ -21155,7 +21155,7 @@
         </is>
       </c>
       <c r="V259" t="n">
-        <v>0.01585626341576416</v>
+        <v>1.585626341576416</v>
       </c>
     </row>
     <row r="260">
@@ -21235,7 +21235,7 @@
         </is>
       </c>
       <c r="V260" t="n">
-        <v>-0.0207922139459165</v>
+        <v>-2.07922139459165</v>
       </c>
     </row>
     <row r="261">
@@ -21315,7 +21315,7 @@
         </is>
       </c>
       <c r="V261" t="n">
-        <v>-0.002880618503153985</v>
+        <v>-0.2880618503153985</v>
       </c>
     </row>
     <row r="262">
@@ -21395,7 +21395,7 @@
         </is>
       </c>
       <c r="V262" t="n">
-        <v>-0.01931705475497852</v>
+        <v>-1.931705475497852</v>
       </c>
     </row>
     <row r="263">
@@ -21475,7 +21475,7 @@
         </is>
       </c>
       <c r="V263" t="n">
-        <v>-0.0208606259549939</v>
+        <v>-2.08606259549939</v>
       </c>
     </row>
     <row r="264">
@@ -21555,7 +21555,7 @@
         </is>
       </c>
       <c r="V264" t="n">
-        <v>-0.005731626638565167</v>
+        <v>-0.5731626638565167</v>
       </c>
     </row>
     <row r="265">
@@ -21635,7 +21635,7 @@
         </is>
       </c>
       <c r="V265" t="n">
-        <v>-0.04633456938681019</v>
+        <v>-4.63345693868102</v>
       </c>
     </row>
     <row r="266">
@@ -21715,7 +21715,7 @@
         </is>
       </c>
       <c r="V266" t="n">
-        <v>-0.02317533386011708</v>
+        <v>-2.317533386011708</v>
       </c>
     </row>
     <row r="267">
@@ -21795,7 +21795,7 @@
         </is>
       </c>
       <c r="V267" t="n">
-        <v>-0.04529113534213297</v>
+        <v>-4.529113534213297</v>
       </c>
     </row>
     <row r="268">
@@ -21875,7 +21875,7 @@
         </is>
       </c>
       <c r="V268" t="n">
-        <v>-0.03738061937405997</v>
+        <v>-3.738061937405996</v>
       </c>
     </row>
     <row r="269">
@@ -21955,7 +21955,7 @@
         </is>
       </c>
       <c r="V269" t="n">
-        <v>-0.0264291854957057</v>
+        <v>-2.64291854957057</v>
       </c>
     </row>
     <row r="270">
@@ -22035,7 +22035,7 @@
         </is>
       </c>
       <c r="V270" t="n">
-        <v>-0.04036128828002452</v>
+        <v>-4.036128828002451</v>
       </c>
     </row>
     <row r="271">
@@ -22115,7 +22115,7 @@
         </is>
       </c>
       <c r="V271" t="n">
-        <v>-0.067976987227356</v>
+        <v>-6.7976987227356</v>
       </c>
     </row>
     <row r="272">
@@ -22195,7 +22195,7 @@
         </is>
       </c>
       <c r="V272" t="n">
-        <v>-0.02231292282577077</v>
+        <v>-2.231292282577077</v>
       </c>
     </row>
     <row r="273">
@@ -22275,7 +22275,7 @@
         </is>
       </c>
       <c r="V273" t="n">
-        <v>-0.03298839822316191</v>
+        <v>-3.298839822316191</v>
       </c>
     </row>
     <row r="274">
@@ -22355,7 +22355,7 @@
         </is>
       </c>
       <c r="V274" t="n">
-        <v>-0.02273719036719601</v>
+        <v>-2.273719036719601</v>
       </c>
     </row>
     <row r="275">
@@ -22435,7 +22435,7 @@
         </is>
       </c>
       <c r="V275" t="n">
-        <v>-0.0228231134136994</v>
+        <v>-2.28231134136994</v>
       </c>
     </row>
     <row r="276">
@@ -22515,7 +22515,7 @@
         </is>
       </c>
       <c r="V276" t="n">
-        <v>-0.08406414823419277</v>
+        <v>-8.406414823419276</v>
       </c>
     </row>
     <row r="277">
@@ -22595,7 +22595,7 @@
         </is>
       </c>
       <c r="V277" t="n">
-        <v>-0.02623870675780129</v>
+        <v>-2.623870675780129</v>
       </c>
     </row>
     <row r="278">
@@ -22675,7 +22675,7 @@
         </is>
       </c>
       <c r="V278" t="n">
-        <v>-0.01865313216588569</v>
+        <v>-1.865313216588569</v>
       </c>
     </row>
     <row r="279">
@@ -22755,7 +22755,7 @@
         </is>
       </c>
       <c r="V279" t="n">
-        <v>-0.03906331702109671</v>
+        <v>-3.906331702109672</v>
       </c>
     </row>
     <row r="280">
@@ -22835,7 +22835,7 @@
         </is>
       </c>
       <c r="V280" t="n">
-        <v>-0.04830500916842228</v>
+        <v>-4.830500916842228</v>
       </c>
     </row>
     <row r="281">
@@ -22915,7 +22915,7 @@
         </is>
       </c>
       <c r="V281" t="n">
-        <v>-0.03255673602257186</v>
+        <v>-3.255673602257186</v>
       </c>
     </row>
     <row r="282">
@@ -22995,7 +22995,7 @@
         </is>
       </c>
       <c r="V282" t="n">
-        <v>-0.03644338648707154</v>
+        <v>-3.644338648707154</v>
       </c>
     </row>
     <row r="283">
@@ -23075,7 +23075,7 @@
         </is>
       </c>
       <c r="V283" t="n">
-        <v>-0.009798579793105633</v>
+        <v>-0.9798579793105634</v>
       </c>
     </row>
     <row r="284">
@@ -23155,7 +23155,7 @@
         </is>
       </c>
       <c r="V284" t="n">
-        <v>-0.01835046594859003</v>
+        <v>-1.835046594859003</v>
       </c>
     </row>
     <row r="285">
@@ -23235,7 +23235,7 @@
         </is>
       </c>
       <c r="V285" t="n">
-        <v>0.01849299127217318</v>
+        <v>1.849299127217318</v>
       </c>
     </row>
     <row r="286">
@@ -23315,7 +23315,7 @@
         </is>
       </c>
       <c r="V286" t="n">
-        <v>-0.0646746990789292</v>
+        <v>-6.467469907892919</v>
       </c>
     </row>
     <row r="287">
@@ -23395,7 +23395,7 @@
         </is>
       </c>
       <c r="V287" t="n">
-        <v>-0.01827276004698613</v>
+        <v>-1.827276004698613</v>
       </c>
     </row>
     <row r="288">
@@ -23475,7 +23475,7 @@
         </is>
       </c>
       <c r="V288" t="n">
-        <v>-0.03734909014500554</v>
+        <v>-3.734909014500554</v>
       </c>
     </row>
     <row r="289">
@@ -23555,7 +23555,7 @@
         </is>
       </c>
       <c r="V289" t="n">
-        <v>-0.02714802558596018</v>
+        <v>-2.714802558596018</v>
       </c>
     </row>
     <row r="290">
@@ -23635,7 +23635,7 @@
         </is>
       </c>
       <c r="V290" t="n">
-        <v>-0.02802969736520524</v>
+        <v>-2.802969736520524</v>
       </c>
     </row>
     <row r="291">
@@ -23715,7 +23715,7 @@
         </is>
       </c>
       <c r="V291" t="n">
-        <v>-0.03893026409366943</v>
+        <v>-3.893026409366943</v>
       </c>
     </row>
   </sheetData>

</xml_diff>